<commit_message>
Added employement data to exampledata2
</commit_message>
<xml_diff>
--- a/starter-analysis-exercise/data/raw-data/exampledata.xlsx
+++ b/starter-analysis-exercise/data/raw-data/exampledata.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA1B0400-91DC-4479-905F-9A91D902E8D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{757C07A3-4880-D643-89F6-498C5C1DC4F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3555" yWindow="945" windowWidth="48840" windowHeight="21645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -115,9 +115,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,15 +401,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -416,8 +419,10 @@
       <c r="C1" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="2"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>180</v>
       </c>
@@ -428,7 +433,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>175</v>
       </c>
@@ -439,7 +444,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -450,7 +455,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>178</v>
       </c>
@@ -461,7 +466,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>192</v>
       </c>
@@ -472,7 +477,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -483,7 +488,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>156</v>
       </c>
@@ -494,7 +499,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>166</v>
       </c>
@@ -505,7 +510,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>155</v>
       </c>
@@ -516,7 +521,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>145</v>
       </c>
@@ -527,7 +532,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>165</v>
       </c>
@@ -535,7 +540,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>133</v>
       </c>
@@ -546,7 +551,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>166</v>
       </c>
@@ -557,7 +562,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>154</v>
       </c>
@@ -578,17 +583,17 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -599,7 +604,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -610,7 +615,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -621,7 +626,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>

</xml_diff>